<commit_message>
IR drivers for different equipment are added to project folder. Not in use. UserDB files are used in compiled code
</commit_message>
<xml_diff>
--- a/Documents/IP_Range - Copy.xlsx
+++ b/Documents/IP_Range - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://srwelectrics-my.sharepoint.com/personal/dan_andrews_srw-group_co_uk/Documents/SRW-Shared/Programming/1 NineElms Amenities/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntaga\Coding\CRESTRON\UK_One9Elms_Crestron\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D78148F-F6DB-4B86-AC53-EFB5C7D138A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3327575E-FE3F-4EFE-9BA1-EFE4F9C32DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="12683" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="384">
   <si>
     <t>network</t>
   </si>
@@ -759,9 +759,6 @@
     <t>10.160.115.217</t>
   </si>
   <si>
-    <t>CP4 or VC4 ?</t>
-  </si>
-  <si>
     <t>10.160.115.218</t>
   </si>
   <si>
@@ -1162,6 +1159,21 @@
   </si>
   <si>
     <t>DIN-AP2</t>
+  </si>
+  <si>
+    <t>New CP4 from Aug 11th 2025</t>
+  </si>
+  <si>
+    <t>Processor Pass</t>
+  </si>
+  <si>
+    <t>Crestron CEN-IO</t>
+  </si>
+  <si>
+    <t>10.160.115.116</t>
+  </si>
+  <si>
+    <t>SAMSUNG</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1264,6 +1276,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1539,22 +1555,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.1328125" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="33.73046875" customWidth="1"/>
+    <col min="6" max="6" width="32.3984375" customWidth="1"/>
+    <col min="7" max="7" width="27.73046875" customWidth="1"/>
+    <col min="10" max="10" width="11.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1685,13 +1701,13 @@
         <v>121</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>122</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>124</v>
@@ -1739,7 +1755,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>34</v>
@@ -1879,7 +1895,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>34</v>
@@ -2103,13 +2119,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C33" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>377</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -2297,49 +2313,37 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
+    <row r="46" spans="1:6">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>365</v>
+      </c>
+      <c r="B48" t="s">
+        <v>378</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="B47" t="s">
-        <v>379</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>122</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>124</v>
@@ -2348,16 +2352,18 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:7">
       <c r="A50" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B50" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>351</v>
+      </c>
       <c r="C50" s="3" t="s">
-        <v>76</v>
+        <v>122</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>124</v>
@@ -2366,16 +2372,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:7">
       <c r="A51" s="3" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>128</v>
+        <v>76</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>124</v>
@@ -2383,8 +2389,11 @@
       <c r="F51" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="3" t="s">
         <v>109</v>
       </c>
@@ -2393,7 +2402,7 @@
         <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>124</v>
@@ -2402,16 +2411,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:7">
       <c r="A53" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>124</v>
@@ -2420,7 +2429,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:7">
       <c r="A54" s="3" t="s">
         <v>130</v>
       </c>
@@ -2429,7 +2438,7 @@
         <v>131</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>124</v>
@@ -2438,16 +2447,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:7">
       <c r="A55" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>124</v>
@@ -2456,7 +2465,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:7">
       <c r="A56" s="3" t="s">
         <v>134</v>
       </c>
@@ -2465,7 +2474,7 @@
         <v>135</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>124</v>
@@ -2474,16 +2483,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:7">
       <c r="A57" s="3" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>124</v>
@@ -2492,16 +2501,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:7">
       <c r="A58" s="3" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>124</v>
@@ -2510,7 +2519,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:7">
       <c r="A59" s="3" t="s">
         <v>19</v>
       </c>
@@ -2519,7 +2528,7 @@
         <v>20</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>124</v>
@@ -2528,16 +2537,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:7">
       <c r="A60" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>124</v>
@@ -2546,16 +2555,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:7">
       <c r="A61" s="3" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>143</v>
+        <v>16</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>124</v>
@@ -2564,52 +2573,54 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:7">
       <c r="A62" s="3" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>365</v>
+        <v>124</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:7">
       <c r="A63" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B63" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>383</v>
+      </c>
       <c r="C63" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>148</v>
+        <v>364</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:7">
       <c r="A64" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>148</v>
@@ -2620,14 +2631,14 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="3" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>148</v>
@@ -2638,14 +2649,14 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="3" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>154</v>
+        <v>16</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>148</v>
@@ -2663,7 +2674,7 @@
         <v>146</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>148</v>
@@ -2674,110 +2685,98 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>350</v>
+        <v>148</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>125</v>
       </c>
     </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="3" t="s">
-        <v>157</v>
-      </c>
+      <c r="A70" s="11"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>159</v>
+        <v>381</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>382</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G71" s="3"/>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G72" s="3"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="12"/>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G73" s="3"/>
+      <c r="G73" s="3" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="3" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>170</v>
+        <v>135</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>163</v>
@@ -2789,14 +2788,14 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="3" t="s">
-        <v>168</v>
+        <v>109</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="3" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>163</v>
@@ -2808,14 +2807,14 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="3" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>163</v>
@@ -2827,14 +2826,14 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="3" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>174</v>
+        <v>169</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>163</v>
@@ -2842,20 +2841,18 @@
       <c r="F77" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>343</v>
-      </c>
+      <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="3" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="3" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>163</v>
@@ -2867,14 +2864,14 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="3" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>176</v>
+        <v>122</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>163</v>
@@ -2885,189 +2882,188 @@
       <c r="G79" s="3"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D80" s="3"/>
-      <c r="E80" s="4" t="s">
+      <c r="A80" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F80" s="1" t="s">
         <v>161</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>178</v>
+        <v>342</v>
       </c>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D81" s="3"/>
-      <c r="E81" s="4" t="s">
+      <c r="A81" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F81" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>178</v>
-      </c>
+      <c r="G81" s="3"/>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="3" t="s">
-        <v>149</v>
+        <v>62</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="E82" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="F82" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G82" s="3" t="s">
-        <v>342</v>
-      </c>
+      <c r="G82" s="3"/>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="C83" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>368</v>
-      </c>
+      <c r="A83" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D83" s="3"/>
       <c r="E83" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="F83" s="5" t="s">
         <v>161</v>
       </c>
+      <c r="G83" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="F84" s="2"/>
+      <c r="A84" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E85" s="3"/>
+      <c r="F85" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="B85" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="C85" s="7"/>
-      <c r="D85" s="6" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="7" customFormat="1">
-      <c r="A86" s="6" t="s">
+      <c r="C88" s="7"/>
+      <c r="D88" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="7" customFormat="1">
+      <c r="A89" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B89" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C89" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D89" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E89" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="F86" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F89" s="1" t="s">
+      <c r="F89" s="8" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>187</v>
+        <v>31</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>182</v>
@@ -3075,19 +3071,19 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>182</v>
@@ -3095,19 +3091,19 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="3" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>182</v>
@@ -3115,19 +3111,19 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>191</v>
+        <v>42</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>182</v>
@@ -3135,19 +3131,19 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>182</v>
@@ -3155,19 +3151,19 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>182</v>
@@ -3175,19 +3171,19 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>195</v>
+        <v>37</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>182</v>
@@ -3195,70 +3191,76 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E97" s="3"/>
+        <v>193</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="F97" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E98" s="3"/>
+        <v>194</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="F98" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="3" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="E99" s="3"/>
+        <v>195</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="F99" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="1" t="s">
@@ -3267,16 +3269,16 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="3" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="1" t="s">
@@ -3285,16 +3287,16 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="3" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>202</v>
+        <v>76</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>199</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="1" t="s">
@@ -3303,16 +3305,16 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="3" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="1" t="s">
@@ -3321,16 +3323,16 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="1" t="s">
@@ -3339,44 +3341,61 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="B105" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="C105" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>349</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E105" s="3"/>
       <c r="F105" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="3" t="s">
-        <v>362</v>
+        <v>44</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>363</v>
+        <v>88</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="F106" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E106" s="3"/>
+      <c r="F106" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="107" spans="1:7">
-      <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="F107" s="1"/>
+      <c r="A107" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E107" s="3"/>
+      <c r="F107" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="3" t="s">
@@ -3386,76 +3405,56 @@
         <v>348</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B109" s="3"/>
+        <v>361</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>362</v>
+      </c>
       <c r="C109" s="3" t="s">
-        <v>76</v>
+        <v>362</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G109" s="3"/>
+        <v>363</v>
+      </c>
+      <c r="F109" s="1"/>
     </row>
     <row r="110" spans="1:7">
-      <c r="A110" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="A110" s="3"/>
       <c r="B110" s="3"/>
-      <c r="C110" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="3" t="s">
-        <v>15</v>
+        <v>345</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>206</v>
+        <v>122</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>347</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G111" s="3"/>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="3" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>212</v>
+        <v>76</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>206</v>
@@ -3467,14 +3466,14 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="3" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>210</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>206</v>
@@ -3486,14 +3485,14 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="3" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>206</v>
@@ -3505,14 +3504,14 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="3" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="3" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>206</v>
@@ -3520,95 +3519,94 @@
       <c r="F115" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G115" s="3" t="s">
-        <v>216</v>
-      </c>
+      <c r="G115" s="3"/>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="3" t="s">
-        <v>149</v>
+        <v>62</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="E116" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="F116" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G116" s="3"/>
     </row>
+    <row r="117" spans="1:7">
+      <c r="A117" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G117" s="3"/>
+    </row>
     <row r="118" spans="1:7">
       <c r="A118" s="3" t="s">
-        <v>346</v>
+        <v>19</v>
       </c>
       <c r="B118" s="3"/>
       <c r="C118" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>347</v>
+        <v>20</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>220</v>
+        <v>207</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="3" t="s">
-        <v>345</v>
+        <v>149</v>
       </c>
       <c r="B119" s="3"/>
       <c r="C119" s="3" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>219</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="E119" s="3"/>
       <c r="F119" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G120" s="3"/>
+        <v>207</v>
+      </c>
+      <c r="G119" s="3"/>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="3" t="s">
-        <v>208</v>
+        <v>345</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="3" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>222</v>
+        <v>346</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>219</v>
@@ -3616,18 +3614,17 @@
       <c r="F121" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G121" s="3"/>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="3" t="s">
-        <v>49</v>
+        <v>344</v>
       </c>
       <c r="B122" s="3"/>
       <c r="C122" s="3" t="s">
-        <v>51</v>
+        <v>122</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>219</v>
@@ -3635,18 +3632,20 @@
       <c r="F122" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G122" s="3"/>
+      <c r="G122" s="3" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B123" s="3"/>
       <c r="C123" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>224</v>
+        <v>76</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>219</v>
@@ -3658,14 +3657,14 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="3" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>227</v>
+        <v>209</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>219</v>
@@ -3677,14 +3676,14 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="3" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>228</v>
+        <v>51</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>223</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>219</v>
@@ -3696,16 +3695,18 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="3" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="E126" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="F126" s="1" t="s">
         <v>220</v>
       </c>
@@ -3713,16 +3714,18 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="3" t="s">
-        <v>15</v>
+        <v>225</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3" t="s">
-        <v>16</v>
+        <v>226</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="E127" s="3"/>
+        <v>227</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="F127" s="1" t="s">
         <v>220</v>
       </c>
@@ -3730,31 +3733,33 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="3" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="B128" s="3"/>
       <c r="C128" s="3" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E128" s="3"/>
+        <v>228</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="F128" s="1" t="s">
         <v>220</v>
       </c>
       <c r="G128" s="3"/>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:8">
       <c r="A129" s="3" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
       <c r="B129" s="3"/>
       <c r="C129" s="3" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E129" s="3"/>
       <c r="F129" s="1" t="s">
@@ -3762,113 +3767,105 @@
       </c>
       <c r="G129" s="3"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:8">
       <c r="A130" s="3" t="s">
-        <v>234</v>
+        <v>15</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="3" t="s">
-        <v>235</v>
+        <v>16</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E130" s="3"/>
       <c r="F130" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G130" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7">
+      <c r="G130" s="3"/>
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131" s="3" t="s">
-        <v>234</v>
+        <v>15</v>
       </c>
       <c r="B131" s="3"/>
       <c r="C131" s="3" t="s">
-        <v>235</v>
+        <v>16</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E131" s="3"/>
       <c r="F131" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G131" s="3" t="s">
+      <c r="G131" s="3"/>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E132" s="3"/>
+      <c r="F132" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G132" s="3"/>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E133" s="3"/>
+      <c r="F133" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G133" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:8">
       <c r="A134" s="3" t="s">
-        <v>49</v>
+        <v>234</v>
       </c>
       <c r="B134" s="3"/>
       <c r="C134" s="3" t="s">
-        <v>51</v>
+        <v>235</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>206</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="E134" s="3"/>
       <c r="F134" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G134" s="3"/>
-    </row>
-    <row r="135" spans="1:7">
-      <c r="A135" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B135" s="3"/>
-      <c r="C135" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E135" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G135" s="3"/>
-    </row>
-    <row r="136" spans="1:7">
-      <c r="A136" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B136" s="3"/>
-      <c r="C136" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7">
+        <v>220</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
       <c r="A137" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B137" s="3"/>
       <c r="C137" s="3" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>206</v>
@@ -3878,16 +3875,16 @@
       </c>
       <c r="G137" s="3"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:8">
       <c r="A138" s="3" t="s">
-        <v>130</v>
+        <v>19</v>
       </c>
       <c r="B138" s="3"/>
       <c r="C138" s="3" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>206</v>
@@ -3897,16 +3894,16 @@
       </c>
       <c r="G138" s="3"/>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:8">
       <c r="A139" s="3" t="s">
-        <v>15</v>
+        <v>242</v>
       </c>
       <c r="B139" s="3"/>
       <c r="C139" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>206</v>
@@ -3914,105 +3911,175 @@
       <c r="F139" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G139" s="3"/>
-    </row>
-    <row r="140" spans="1:7">
-      <c r="A140" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B140" s="4"/>
-      <c r="C140" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D140" s="3"/>
-      <c r="E140" s="4" t="s">
+      <c r="G139" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="H139" s="10" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E140" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F140" s="5" t="s">
+      <c r="F140" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G140" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7">
+      <c r="G140" s="3"/>
+    </row>
+    <row r="141" spans="1:8">
       <c r="A141" s="3" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B141" s="3"/>
       <c r="C141" s="3" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="E141" s="3"/>
+        <v>246</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="F141" s="1" t="s">
         <v>240</v>
       </c>
       <c r="G141" s="3"/>
     </row>
-    <row r="143" spans="1:7">
-      <c r="A143" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B143" s="3"/>
-      <c r="C143" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="E143" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>254</v>
+    <row r="142" spans="1:8">
+      <c r="A142" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G142" s="3"/>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D143" s="3"/>
+      <c r="E143" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F143" s="5" t="s">
+        <v>240</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
       <c r="A144" s="3" t="s">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="B144" s="3"/>
       <c r="C144" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E144" s="3"/>
+      <c r="F144" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G144" s="3"/>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B146" s="3"/>
+      <c r="C146" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D146" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="E146" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B147" s="3"/>
+      <c r="C147" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E147" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E144" s="3" t="s">
+      <c r="F147" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D148" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="F144" s="1" t="s">
+      <c r="E148" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G148" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="G144" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7">
-      <c r="A145" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B145" s="3"/>
-      <c r="C145" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G145" s="3" t="s">
-        <v>255</v>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="F156" t="s">
+        <v>380</v>
+      </c>
+      <c r="G156">
+        <v>4719124719</v>
       </c>
     </row>
   </sheetData>
@@ -4029,13 +4096,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.3984375" customWidth="1"/>
+    <col min="3" max="3" width="22.265625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" customWidth="1"/>
+    <col min="6" max="6" width="27.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4043,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4051,7 +4118,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4067,7 +4134,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4095,16 +4162,16 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>39</v>
@@ -4115,16 +4182,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>27</v>
@@ -4135,19 +4202,19 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>275</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>28</v>
@@ -4155,19 +4222,19 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>28</v>
@@ -4175,16 +4242,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>55</v>
@@ -4195,16 +4262,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
@@ -4222,7 +4289,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
@@ -4231,16 +4298,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>284</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
@@ -4258,7 +4325,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>97</v>
@@ -4278,7 +4345,7 @@
         <v>103</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>97</v>
@@ -4298,7 +4365,7 @@
         <v>107</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>97</v>
@@ -4309,16 +4376,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>181</v>
@@ -4329,16 +4396,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>265</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>186</v>
@@ -4349,19 +4416,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>273</v>
-      </c>
       <c r="D22" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>291</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>182</v>
@@ -4369,16 +4436,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>192</v>
@@ -4389,16 +4456,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="1" t="s">
@@ -4416,7 +4483,7 @@
         <v>84</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="1" t="s">
@@ -4425,16 +4492,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="1" t="s">
@@ -4454,13 +4521,13 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.265625" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" customWidth="1"/>
+    <col min="4" max="4" width="21.73046875" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" customWidth="1"/>
+    <col min="6" max="6" width="32.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4468,7 +4535,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4476,7 +4543,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4492,7 +4559,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4520,16 +4587,16 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>301</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -4546,7 +4613,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>27</v>
@@ -4558,16 +4625,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>302</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>27</v>
@@ -4578,16 +4645,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>39</v>
@@ -4598,19 +4665,19 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>308</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>28</v>
@@ -4618,16 +4685,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>61</v>
@@ -4638,16 +4705,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>311</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>312</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>55</v>
@@ -4667,7 +4734,7 @@
         <v>80</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="1" t="s">
@@ -4679,14 +4746,14 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>316</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>124</v>
@@ -4697,14 +4764,14 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>124</v>
@@ -4715,14 +4782,14 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>124</v>
@@ -4733,14 +4800,14 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>124</v>
@@ -4751,14 +4818,14 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>322</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>148</v>
@@ -4769,14 +4836,14 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>148</v>
@@ -4787,14 +4854,14 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>148</v>
@@ -4805,17 +4872,17 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>326</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>125</v>
@@ -4823,14 +4890,14 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>160</v>
@@ -4841,14 +4908,14 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>163</v>
@@ -4862,16 +4929,16 @@
     </row>
     <row r="29" spans="1:7" s="7" customFormat="1">
       <c r="A29" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>360</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>361</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>186</v>
@@ -4882,16 +4949,16 @@
     </row>
     <row r="30" spans="1:7" s="7" customFormat="1">
       <c r="A30" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>301</v>
-      </c>
       <c r="D30" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>186</v>
@@ -4905,16 +4972,16 @@
     </row>
     <row r="31" spans="1:7" s="7" customFormat="1">
       <c r="A31" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>301</v>
-      </c>
       <c r="D31" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>181</v>
@@ -4925,16 +4992,16 @@
     </row>
     <row r="32" spans="1:7" s="7" customFormat="1">
       <c r="A32" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>305</v>
-      </c>
       <c r="D32" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>186</v>
@@ -4943,21 +5010,21 @@
         <v>182</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="7" customFormat="1">
       <c r="A33" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>192</v>
@@ -4968,35 +5035,35 @@
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1">
       <c r="A34" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="8" t="s">
         <v>182</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>219</v>
@@ -5007,14 +5074,14 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>219</v>
@@ -5025,14 +5092,14 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>219</v>
@@ -5051,14 +5118,14 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="1" t="s">
@@ -5067,14 +5134,14 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>338</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="1" t="s">
@@ -5083,14 +5150,14 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="1" t="s">
@@ -5106,7 +5173,7 @@
         <v>235</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="1" t="s">
@@ -5122,7 +5189,7 @@
         <v>235</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="1" t="s">

</xml_diff>